<commit_message>
Distance File: Don't output non-square matrices
</commit_message>
<xml_diff>
--- a/Orange/tests/xlsx_files/distances_with_nans.xlsx
+++ b/Orange/tests/xlsx_files/distances_with_nans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janez/orange3/Orange/tests/xlsx_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A438DE-0110-8C41-A9F5-1205412F5D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369761CD-19AC-C542-8978-8503C985549F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -389,17 +389,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>